<commit_message>
Update scrum for sprint 2
</commit_message>
<xml_diff>
--- a/docs/Scrum.xlsx
+++ b/docs/Scrum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -297,7 +297,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
   <si>
     <t xml:space="preserve">Last Update</t>
   </si>
@@ -508,7 +508,13 @@
     <t xml:space="preserve">Currency details (Jeremiah, Steve)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dashboard (Kenneth, whoever)</t>
+    <t xml:space="preserve">Dashboard (Kenneth, Jeremiah)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange rate configuration (Steve)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange rate calculator (Steve)</t>
   </si>
   <si>
     <t xml:space="preserve">User account (Patrick, Jaymar)</t>
@@ -523,6 +529,9 @@
     <t xml:space="preserve">Currency filtering (Steve)</t>
   </si>
   <si>
+    <t xml:space="preserve">Currency sorting (Jeremiah)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sprint ID</t>
   </si>
   <si>
@@ -532,28 +541,22 @@
     <t xml:space="preserve">Tasks Completed</t>
   </si>
   <si>
-    <t xml:space="preserve">David Hoffman</t>
+    <t xml:space="preserve">Jeremiah</t>
   </si>
   <si>
-    <t xml:space="preserve">Task 1: Login Page Design (John Li)</t>
+    <t xml:space="preserve">Task 5: Currency list</t>
   </si>
   <si>
-    <t xml:space="preserve">Task ?</t>
+    <t xml:space="preserve">Task 6: Currency filtering</t>
   </si>
   <si>
-    <t xml:space="preserve">..</t>
+    <t xml:space="preserve">Completed</t>
   </si>
   <si>
-    <t xml:space="preserve">Story Points (Total)</t>
+    <t xml:space="preserve">Accumulated</t>
   </si>
   <si>
-    <t xml:space="preserve">Story Points (Completed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Story Points (Accumulated)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Story Points (Remaining)</t>
+    <t xml:space="preserve">Remaining</t>
   </si>
   <si>
     <t xml:space="preserve">Ideal</t>
@@ -923,7 +926,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -941,7 +944,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Story Points (Remaining)</c:v>
+                  <c:v>Remaining</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -961,6 +964,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -972,6 +976,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -981,71 +986,35 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$2:$A$10</c:f>
+              <c:f>'Burndown Chart'!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$E$2:$E$10</c:f>
+              <c:f>'Burndown Chart'!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
+                  <c:v>43.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1081,6 +1050,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1092,6 +1062,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1101,71 +1072,35 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$2:$A$10</c:f>
+              <c:f>'Burndown Chart'!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$F$2:$F$10</c:f>
+              <c:f>'Burndown Chart'!$F$2:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.625</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21.875</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13.125</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.75</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.375</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1180,11 +1115,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="37973183"/>
-        <c:axId val="8412775"/>
+        <c:axId val="6071675"/>
+        <c:axId val="46348292"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37973183"/>
+        <c:axId val="6071675"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,14 +1145,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8412775"/>
+        <c:crossAx val="46348292"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8412775"/>
+        <c:axId val="46348292"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35"/>
@@ -1254,7 +1189,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37973183"/>
+        <c:crossAx val="6071675"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1290,7 +1225,9 @@
     <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
-    <a:noFill/>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
@@ -1303,15 +1240,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>57240</xdr:rowOff>
+      <xdr:colOff>49680</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>181440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>429480</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>689760</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1319,8 +1256,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="594720" y="2057400"/>
-        <a:ext cx="3362040" cy="2076120"/>
+        <a:off x="925200" y="948960"/>
+        <a:ext cx="3364200" cy="2079720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6443,7 +6380,7 @@
   </sheetPr>
   <dimension ref="A1:F1006"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
@@ -13679,10 +13616,10 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13708,46 +13645,45 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="25" t="s">
         <v>66</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
-        <v>38</v>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="25" t="s">
+        <v>68</v>
       </c>
-      <c r="B5" s="7"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
-        <v>40</v>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="25" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13755,14 +13691,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="25" t="s">
-        <v>71</v>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="25" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
-        <v>52</v>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="24" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13802,7 +13738,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13815,47 +13751,41 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>78</v>
-      </c>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="24"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24"/>
@@ -16862,213 +16792,119 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>35</v>
+        <v>43.5</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>35</v>
+        <f aca="false">B2-C2+D2</f>
+        <v>35.5</v>
       </c>
       <c r="F2" s="7" t="n">
-        <v>35</v>
+        <f aca="false">B2-C2</f>
+        <v>35.5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7" t="n">
-        <v>35</v>
+        <f aca="false">B2+D2</f>
+        <v>43.5</v>
       </c>
       <c r="C3" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7" t="n">
-        <f aca="false">C3</f>
-        <v>2</v>
+        <v>0</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">B3-D3</f>
-        <v>33</v>
+      <c r="E3" s="7" t="n">
+        <f aca="false">B3-C3+D3</f>
+        <v>43.5</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <f aca="false">35-35/8*A3</f>
-        <v>30.625</v>
+      <c r="F3" s="7" t="n">
+        <f aca="false">B3-C3</f>
+        <v>43.5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="n">
-        <v>36</v>
+        <f aca="false">B3+D3</f>
+        <v>43.5</v>
       </c>
       <c r="C4" s="7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" s="7" t="n">
-        <f aca="false">SUM(C3:C4)</f>
-        <v>5</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <f aca="false">B4-D4</f>
-        <v>31</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <f aca="false">35-35/8*A4</f>
-        <v>26.25</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>36</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">SUM(C3:C5)</f>
-        <v>8</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <f aca="false">B5-D5</f>
-        <v>28</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <f aca="false">35-35/8*A5</f>
-        <v>21.875</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>36</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <f aca="false">SUM(C3:C6)</f>
-        <v>12</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <f aca="false">B6-D6</f>
-        <v>24</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <f aca="false">35-35/8*A6</f>
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>34</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">SUM(C3:C7)</f>
-        <v>15</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <f aca="false">B7-D7</f>
-        <v>19</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <f aca="false">35-35/8*A7</f>
-        <v>13.125</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="F8" s="0" t="n">
-        <f aca="false">35-35/8*A8</f>
-        <v>8.75</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="F9" s="0" t="n">
-        <f aca="false">35-35/8*A9</f>
-        <v>4.375</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="F10" s="0" t="n">
-        <f aca="false">35-35/8*A10</f>
         <v>0</v>
       </c>
-    </row>
+      <c r="E4" s="7" t="n">
+        <f aca="false">B4-C4+D4</f>
+        <v>43.5</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <f aca="false">B4-C4</f>
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update scrum sheet for sprint 2
</commit_message>
<xml_diff>
--- a/docs/Scrum.xlsx
+++ b/docs/Scrum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -244,60 +244,8 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="D5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Implement the DB with SQLite based on the design of account table
-Acceptance Criteria:
-1. XXX
-2. XXX
-Verified by: John Li</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="C2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Design the login page, including the registration link</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t xml:space="preserve">Last Update</t>
   </si>
@@ -511,6 +459,12 @@
     <t xml:space="preserve">Dashboard (Kenneth, whoever)</t>
   </si>
   <si>
+    <t xml:space="preserve">Exchange rate configuration (Steve)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange rate calculator (Steve)</t>
+  </si>
+  <si>
     <t xml:space="preserve">User account (Patrick, Jaymar)</t>
   </si>
   <si>
@@ -523,6 +477,9 @@
     <t xml:space="preserve">Currency filtering (Steve)</t>
   </si>
   <si>
+    <t xml:space="preserve">Currency sorting (Jeremiah)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sprint ID</t>
   </si>
   <si>
@@ -530,18 +487,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tasks Completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Hoffman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task 1: Login Page Design (John Li)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">..</t>
   </si>
   <si>
     <t xml:space="preserve">Story Points (Total)</t>
@@ -726,7 +671,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -847,6 +792,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -923,7 +872,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -961,6 +910,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -972,6 +922,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -981,71 +932,35 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$2:$A$10</c:f>
+              <c:f>'Burndown Chart'!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$E$2:$E$10</c:f>
+              <c:f>'Burndown Chart'!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
+                  <c:v>20.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1081,6 +996,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1092,6 +1008,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1101,70 +1018,34 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$2:$A$10</c:f>
+              <c:f>'Burndown Chart'!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$F$2:$F$10</c:f>
+              <c:f>'Burndown Chart'!$F$2:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.625</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21.875</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13.125</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.75</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.375</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1180,11 +1061,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="37973183"/>
-        <c:axId val="8412775"/>
+        <c:axId val="28132167"/>
+        <c:axId val="22153046"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37973183"/>
+        <c:axId val="28132167"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,14 +1091,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8412775"/>
+        <c:crossAx val="22153046"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8412775"/>
+        <c:axId val="22153046"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35"/>
@@ -1254,7 +1135,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37973183"/>
+        <c:crossAx val="28132167"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1303,15 +1184,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>57240</xdr:rowOff>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>429480</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:colOff>429120</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1319,8 +1200,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="594720" y="2057400"/>
-        <a:ext cx="3362040" cy="2076120"/>
+        <a:off x="595080" y="825120"/>
+        <a:ext cx="3359880" cy="2075400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6446,7 +6327,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13679,17 +13560,18 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="39.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="14.43"/>
   </cols>
   <sheetData>
@@ -13708,77 +13590,116 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="25" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="25" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="25" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="30"/>
+      <c r="B4" s="16" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="7"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="25" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="25" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="25" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="25" t="s">
-        <v>71</v>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="16" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
-        <v>52</v>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="25" t="s">
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="16" t="s">
         <v>58</v>
       </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -13788,7 +13709,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13802,78 +13722,102 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>75</v>
+      <c r="B2" s="7"/>
+      <c r="C2" s="16" t="s">
+        <v>65</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>75</v>
+      <c r="B3" s="7"/>
+      <c r="C3" s="16" t="s">
+        <v>66</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>77</v>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="24" t="n">
+        <v>1</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>78</v>
+      <c r="B4" s="7"/>
+      <c r="C4" s="16" t="s">
+        <v>73</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>78</v>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="24" t="n">
+        <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>78</v>
+      <c r="C5" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24"/>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="24"/>
@@ -16853,7 +16797,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16862,18 +16805,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.29"/>
@@ -16882,193 +16825,99 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>72</v>
+      <c r="A1" s="31" t="s">
+        <v>75</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="D1" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="E1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>35</v>
+        <v>43.5</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>35</v>
+        <f aca="false">B2-C2+D2</f>
+        <v>32.5</v>
       </c>
-      <c r="F2" s="7" t="n">
-        <v>35</v>
+      <c r="F2" s="0" t="n">
+        <f aca="false">$B$2-$B$2/3*A2</f>
+        <v>29</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7" t="n">
-        <v>35</v>
+        <f aca="false">E2</f>
+        <v>32.5</v>
       </c>
       <c r="C3" s="7" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D3" s="7" t="n">
-        <f aca="false">C3</f>
-        <v>2</v>
+        <v>0</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">B3-D3</f>
-        <v>33</v>
+      <c r="E3" s="7" t="n">
+        <f aca="false">B3-C3+D3</f>
+        <v>20.5</v>
       </c>
       <c r="F3" s="0" t="n">
-        <f aca="false">35-35/8*A3</f>
-        <v>30.625</v>
+        <f aca="false">$B$2-$B$2/3*A3</f>
+        <v>14.5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="n">
-        <v>36</v>
+        <f aca="false">E3</f>
+        <v>20.5</v>
       </c>
       <c r="C4" s="7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" s="7" t="n">
-        <f aca="false">SUM(C3:C4)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">B4-D4</f>
-        <v>31</v>
+        <v>20.5</v>
       </c>
       <c r="F4" s="0" t="n">
-        <f aca="false">35-35/8*A4</f>
-        <v>26.25</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>36</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">SUM(C3:C5)</f>
-        <v>8</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <f aca="false">B5-D5</f>
-        <v>28</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <f aca="false">35-35/8*A5</f>
-        <v>21.875</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>36</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <f aca="false">SUM(C3:C6)</f>
-        <v>12</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <f aca="false">B6-D6</f>
-        <v>24</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <f aca="false">35-35/8*A6</f>
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>34</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">SUM(C3:C7)</f>
-        <v>15</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <f aca="false">B7-D7</f>
-        <v>19</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <f aca="false">35-35/8*A7</f>
-        <v>13.125</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="F8" s="0" t="n">
-        <f aca="false">35-35/8*A8</f>
-        <v>8.75</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="F9" s="0" t="n">
-        <f aca="false">35-35/8*A9</f>
-        <v>4.375</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="F10" s="0" t="n">
-        <f aca="false">35-35/8*A10</f>
+        <f aca="false">$B$2-$B$2/3*A4</f>
         <v>0</v>
       </c>
     </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update scrum sheet with plan for sprint 3
</commit_message>
<xml_diff>
--- a/docs/Scrum.xlsx
+++ b/docs/Scrum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -245,7 +245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="87">
   <si>
     <t xml:space="preserve">Last Update</t>
   </si>
@@ -456,7 +456,7 @@
     <t xml:space="preserve">Currency details (Jeremiah, Steve)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dashboard (Kenneth, whoever)</t>
+    <t xml:space="preserve">Dashboard (Kenneth, Jeremiah)</t>
   </si>
   <si>
     <t xml:space="preserve">Exchange rate configuration (Steve)</t>
@@ -474,10 +474,22 @@
     <t xml:space="preserve">Registration (Patrick, Jaymar)</t>
   </si>
   <si>
+    <t xml:space="preserve">Push notifications (Jeremiah)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Currency filtering (Steve)</t>
   </si>
   <si>
     <t xml:space="preserve">Currency sorting (Jeremiah)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share menu (Steve)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cryptocurrency news (Patrick, Jaymar)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User commenting (Steve)</t>
   </si>
   <si>
     <t xml:space="preserve">Sprint ID</t>
@@ -671,7 +683,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -798,6 +810,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1061,11 +1077,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="28132167"/>
-        <c:axId val="22153046"/>
+        <c:axId val="62990652"/>
+        <c:axId val="9512014"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="28132167"/>
+        <c:axId val="62990652"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,14 +1107,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22153046"/>
+        <c:crossAx val="9512014"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22153046"/>
+        <c:axId val="9512014"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35"/>
@@ -1135,7 +1151,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28132167"/>
+        <c:crossAx val="62990652"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1184,7 +1200,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>57600</xdr:rowOff>
     </xdr:from>
@@ -1192,7 +1208,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>429120</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1200,8 +1216,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="595080" y="825120"/>
-        <a:ext cx="3359880" cy="2075400"/>
+        <a:off x="595440" y="826560"/>
+        <a:ext cx="3359520" cy="2075040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -13560,16 +13576,16 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="14.43"/>
@@ -13605,7 +13621,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="30"/>
       <c r="B4" s="16" t="s">
         <v>67</v>
@@ -13653,11 +13669,10 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
-        <v>48</v>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="16" t="s">
+        <v>73</v>
       </c>
-      <c r="B10" s="30"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
     </row>
@@ -13666,7 +13681,7 @@
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
       <c r="D11" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13674,30 +13689,27 @@
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
       <c r="D12" s="21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
-        <v>54</v>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="16" t="s">
+        <v>76</v>
       </c>
-      <c r="B13" s="30"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="s">
-        <v>56</v>
+      <c r="B14" s="16" t="s">
+        <v>77</v>
       </c>
-      <c r="B14" s="30"/>
       <c r="C14" s="30"/>
       <c r="D14" s="30"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
-        <v>58</v>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="16" t="s">
+        <v>78</v>
       </c>
-      <c r="B15" s="30"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
     </row>
@@ -13735,13 +13747,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13768,7 +13780,7 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13816,7 +13828,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16807,10 +16819,10 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16826,22 +16838,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16889,7 +16901,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
         <v>3</v>
       </c>
@@ -16903,7 +16915,7 @@
       <c r="D4" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="32" t="n">
         <f aca="false">B4-D4</f>
         <v>20.5</v>
       </c>

</xml_diff>